<commit_message>
Controle Ponto Final v3.0 by RP
</commit_message>
<xml_diff>
--- a/COntrolePontoV3.0Final.xlsx
+++ b/COntrolePontoV3.0Final.xlsx
@@ -819,31 +819,23 @@
       <c r="A6" s="20">
         <v>43770.0</v>
       </c>
-      <c r="B6" s="21">
-        <v>0.2916666666666667</v>
-      </c>
-      <c r="C6" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0.5416666666666666</v>
-      </c>
-      <c r="E6" s="21">
-        <v>0.6666666666666666</v>
-      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="22">
+      <c r="H6" s="22" t="str">
         <f t="shared" ref="H6:H13" si="1">IF(OR(B6&lt;&gt;"",C6&lt;&gt;""),IF(OR(D6="",E6=""),C6-B6,(C6-B6)+(E6-D6)-$L$4),"")</f>
-        <v>0.2916666667</v>
+        <v/>
       </c>
       <c r="I6" s="23" t="str">
         <f t="shared" ref="I6:I35" si="2">IF(OR(G6&lt;&gt;"",E6&lt;&gt;""),IF((H6&lt;$M$4),(H6-$M$4)+(G6-F6),IF(OR(G6&lt;&gt;"",F6&lt;&gt;""),G6-F6,"")),"")</f>
         <v/>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="24" t="str">
         <f t="shared" ref="J6:J35" si="3">IF(OR(H6&lt;&gt;"",I6&lt;&gt;""),IF((I6&gt;$K$2),I6+H6,H6),"")</f>
-        <v>0.2916666667</v>
+        <v/>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
@@ -875,7 +867,7 @@
       </c>
       <c r="M7" s="27">
         <f>SUMIF(I6:I35,"&lt;00:00:00")+M12</f>
-        <v>0.2916666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1005,7 +997,7 @@
       </c>
       <c r="M12" s="33">
         <f>SUM(J6:J35)</f>
-        <v>0.2916666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">

</xml_diff>